<commit_message>
feat: refactor real_data into own function and fix imports
</commit_message>
<xml_diff>
--- a/results/robustness_checks_formatted.xlsx
+++ b/results/robustness_checks_formatted.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\projects\python\bsic_systematic_fx\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC45D692-4452-40A0-B022-E7DE861D2131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94CDE65E-E4E6-416C-A7F1-6039CDA5B29F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="390" windowWidth="28800" windowHeight="15585" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 (2)" sheetId="10" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="9" r:id="rId2"/>
-    <sheet name="format_to_bsic_standards" sheetId="8" r:id="rId3"/>
-    <sheet name="paper_weekly_rebalancing" sheetId="7" r:id="rId4"/>
-    <sheet name="paper" sheetId="6" r:id="rId5"/>
+    <sheet name="paper_weekly_rebalancing" sheetId="7" r:id="rId3"/>
+    <sheet name="paper" sheetId="6" r:id="rId4"/>
+    <sheet name="format_to_bsic_standards" sheetId="8" r:id="rId5"/>
     <sheet name="improved_stats" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
   <si>
     <t>Total</t>
   </si>
@@ -165,7 +165,13 @@
     <t>November 10, 2022 (USD, 000s)</t>
   </si>
   <si>
-    <t>Window / SR</t>
+    <t>SR vs MA Window</t>
+  </si>
+  <si>
+    <t>Period</t>
+  </si>
+  <si>
+    <t>Source: BSIC</t>
   </si>
 </sst>
 </file>
@@ -173,13 +179,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="166" formatCode="#,##0;\(#,##0\)"/>
-    <numFmt numFmtId="167" formatCode="0.0%"/>
-    <numFmt numFmtId="168" formatCode="0.0"/>
-    <numFmt numFmtId="169" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="#,##0;\(#,##0\)"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -285,6 +291,13 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Gill Sans MT"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Gill Sans MT"/>
       <family val="2"/>
     </font>
@@ -452,9 +465,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -480,24 +493,24 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -510,27 +523,24 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="168" fontId="11" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="11" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="5" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -549,7 +559,7 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -568,6 +578,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -968,75 +987,75 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="51"/>
+      <c r="D2" s="50"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="49">
+      <c r="B3" s="48">
         <v>82400</v>
       </c>
-      <c r="C3" s="48">
+      <c r="C3" s="47">
         <v>301440</v>
       </c>
-      <c r="E3" s="50"/>
+      <c r="E3" s="49"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="49">
+      <c r="B4" s="48">
         <v>3180393</v>
       </c>
-      <c r="C4" s="48">
+      <c r="C4" s="47">
         <v>798052.47099150007</v>
       </c>
-      <c r="D4" s="47"/>
+      <c r="D4" s="46"/>
     </row>
     <row r="5" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="46">
+      <c r="B5" s="45">
         <v>2187876.1719999998</v>
       </c>
-      <c r="C5" s="45">
+      <c r="C5" s="44">
         <v>553903.77300000004</v>
       </c>
-      <c r="F5" s="44"/>
-    </row>
-    <row r="6" spans="1:6" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="43" t="s">
+      <c r="F5" s="43"/>
+    </row>
+    <row r="6" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="42">
+      <c r="B6" s="41">
         <f>B$5/B3</f>
         <v>26.551895291262134</v>
       </c>
-      <c r="C6" s="41">
+      <c r="C6" s="40">
         <f>C$5/C3</f>
         <v>1.8375257862261147</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="40" t="s">
+    <row r="7" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="39">
+      <c r="B7" s="38">
         <f>B$5/B4</f>
         <v>0.68792635752877074</v>
       </c>
-      <c r="C7" s="38">
+      <c r="C7" s="37">
         <f>C$5/C4</f>
         <v>0.69406936653153928</v>
       </c>
@@ -1268,44 +1287,44 @@
       </c>
     </row>
     <row r="16" spans="2:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="64"/>
+      <c r="F16" s="64"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
+      <c r="C17" s="64"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="64"/>
     </row>
     <row r="18" spans="2:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
+      <c r="C18" s="64"/>
+      <c r="D18" s="64"/>
+      <c r="E18" s="64"/>
+      <c r="F18" s="64"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="35" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="35" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="35" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1321,224 +1340,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5220731-67A1-4BB6-853C-66EAA50B4340}">
-  <dimension ref="B2:Q5"/>
-  <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:17" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="55" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="56">
-        <v>2</v>
-      </c>
-      <c r="D2" s="56">
-        <v>4</v>
-      </c>
-      <c r="E2" s="56">
-        <v>6</v>
-      </c>
-      <c r="F2" s="56">
-        <v>8</v>
-      </c>
-      <c r="G2" s="56">
-        <v>10</v>
-      </c>
-      <c r="H2" s="56">
-        <v>12</v>
-      </c>
-      <c r="I2" s="56">
-        <v>14</v>
-      </c>
-      <c r="J2" s="56">
-        <v>16</v>
-      </c>
-      <c r="K2" s="56">
-        <v>18</v>
-      </c>
-      <c r="L2" s="56">
-        <v>20</v>
-      </c>
-      <c r="M2" s="56">
-        <v>22</v>
-      </c>
-      <c r="N2" s="56">
-        <v>24</v>
-      </c>
-      <c r="O2" s="56">
-        <v>26</v>
-      </c>
-      <c r="P2" s="56">
-        <v>28</v>
-      </c>
-      <c r="Q2" s="57">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="63" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="59">
-        <v>0.10277109753760059</v>
-      </c>
-      <c r="D3" s="59">
-        <v>0.59300118816030833</v>
-      </c>
-      <c r="E3" s="59">
-        <v>0.57222594432367402</v>
-      </c>
-      <c r="F3" s="59">
-        <v>0.57086164296253339</v>
-      </c>
-      <c r="G3" s="60">
-        <v>0.64180904570128883</v>
-      </c>
-      <c r="H3" s="59">
-        <v>0.61085426480264182</v>
-      </c>
-      <c r="I3" s="59">
-        <v>0.57590467725145278</v>
-      </c>
-      <c r="J3" s="59">
-        <v>0.56236254763286742</v>
-      </c>
-      <c r="K3" s="59">
-        <v>0.57289810690953979</v>
-      </c>
-      <c r="L3" s="59">
-        <v>0.51874473895218609</v>
-      </c>
-      <c r="M3" s="59">
-        <v>0.50603392826946225</v>
-      </c>
-      <c r="N3" s="59">
-        <v>0.45168989992585939</v>
-      </c>
-      <c r="O3" s="59">
-        <v>0.42247144953337212</v>
-      </c>
-      <c r="P3" s="59">
-        <v>0.41177611120618529</v>
-      </c>
-      <c r="Q3" s="61">
-        <v>0.34946955395097867</v>
-      </c>
-    </row>
-    <row r="4" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="64" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="58">
-        <v>1.0490137114163001</v>
-      </c>
-      <c r="D4" s="58">
-        <v>1.434982139485669</v>
-      </c>
-      <c r="E4" s="58">
-        <v>1.2943047991730501</v>
-      </c>
-      <c r="F4" s="58">
-        <v>1.2391795365528739</v>
-      </c>
-      <c r="G4" s="58">
-        <v>1.3694102876617571</v>
-      </c>
-      <c r="H4" s="58">
-        <v>1.443042284823141</v>
-      </c>
-      <c r="I4" s="58">
-        <v>1.3700343552736449</v>
-      </c>
-      <c r="J4" s="58">
-        <v>1.299822883627044</v>
-      </c>
-      <c r="K4" s="58">
-        <v>1.350071627379829</v>
-      </c>
-      <c r="L4" s="58">
-        <v>1.248677773165314</v>
-      </c>
-      <c r="M4" s="58">
-        <v>1.212098843731839</v>
-      </c>
-      <c r="N4" s="58">
-        <v>1.0981818670917001</v>
-      </c>
-      <c r="O4" s="58">
-        <v>1.0119847234027859</v>
-      </c>
-      <c r="P4" s="58">
-        <v>0.99890562562774432</v>
-      </c>
-      <c r="Q4" s="62">
-        <v>0.91153359502956166</v>
-      </c>
-    </row>
-    <row r="5" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="63" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="59">
-        <v>-0.57544962133575761</v>
-      </c>
-      <c r="D5" s="59">
-        <v>-0.19549829188749829</v>
-      </c>
-      <c r="E5" s="59">
-        <v>-0.15163963681265219</v>
-      </c>
-      <c r="F5" s="59">
-        <v>-0.31019878694465541</v>
-      </c>
-      <c r="G5" s="59">
-        <v>-0.27765141209030197</v>
-      </c>
-      <c r="H5" s="59">
-        <v>-0.21299648359270409</v>
-      </c>
-      <c r="I5" s="59">
-        <v>-0.2098310782613807</v>
-      </c>
-      <c r="J5" s="59">
-        <v>-0.1932366748722153</v>
-      </c>
-      <c r="K5" s="59">
-        <v>-0.22183807121746441</v>
-      </c>
-      <c r="L5" s="59">
-        <v>-0.19275918118383559</v>
-      </c>
-      <c r="M5" s="59">
-        <v>-0.17331960112314251</v>
-      </c>
-      <c r="N5" s="59">
-        <v>-0.20620580112628589</v>
-      </c>
-      <c r="O5" s="59">
-        <v>-0.2046546717033354</v>
-      </c>
-      <c r="P5" s="59">
-        <v>-0.20626312632416219</v>
-      </c>
-      <c r="Q5" s="61">
-        <v>-0.23163087276473621</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF2F1E75-5BB3-4BD5-9F5B-C2F7B74DD9A3}">
   <dimension ref="A1:D31"/>
   <sheetViews>
@@ -1984,7 +1785,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16E5077C-487C-40AA-9EB5-A098603EF849}">
   <dimension ref="A1:U30"/>
   <sheetViews>
@@ -2608,12 +2409,277 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5220731-67A1-4BB6-853C-66EAA50B4340}">
+  <dimension ref="B2:S8"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:Q8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:19" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="B2" s="65" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="65"/>
+      <c r="N2" s="65"/>
+      <c r="O2" s="65"/>
+      <c r="P2" s="65"/>
+      <c r="Q2" s="65"/>
+    </row>
+    <row r="3" spans="2:19" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="55">
+        <v>2</v>
+      </c>
+      <c r="D3" s="55">
+        <v>4</v>
+      </c>
+      <c r="E3" s="55">
+        <v>6</v>
+      </c>
+      <c r="F3" s="55">
+        <v>8</v>
+      </c>
+      <c r="G3" s="55">
+        <v>10</v>
+      </c>
+      <c r="H3" s="55">
+        <v>12</v>
+      </c>
+      <c r="I3" s="55">
+        <v>14</v>
+      </c>
+      <c r="J3" s="55">
+        <v>16</v>
+      </c>
+      <c r="K3" s="55">
+        <v>18</v>
+      </c>
+      <c r="L3" s="55">
+        <v>20</v>
+      </c>
+      <c r="M3" s="55">
+        <v>22</v>
+      </c>
+      <c r="N3" s="55">
+        <v>24</v>
+      </c>
+      <c r="O3" s="55">
+        <v>26</v>
+      </c>
+      <c r="P3" s="55">
+        <v>28</v>
+      </c>
+      <c r="Q3" s="56">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="58">
+        <v>0.10277109753760059</v>
+      </c>
+      <c r="D4" s="58">
+        <v>0.59300118816030833</v>
+      </c>
+      <c r="E4" s="58">
+        <v>0.57222594432367402</v>
+      </c>
+      <c r="F4" s="58">
+        <v>0.57086164296253339</v>
+      </c>
+      <c r="G4" s="59">
+        <v>0.64180904570128883</v>
+      </c>
+      <c r="H4" s="58">
+        <v>0.61085426480264182</v>
+      </c>
+      <c r="I4" s="58">
+        <v>0.57590467725145278</v>
+      </c>
+      <c r="J4" s="58">
+        <v>0.56236254763286742</v>
+      </c>
+      <c r="K4" s="58">
+        <v>0.57289810690953979</v>
+      </c>
+      <c r="L4" s="58">
+        <v>0.51874473895218609</v>
+      </c>
+      <c r="M4" s="58">
+        <v>0.50603392826946225</v>
+      </c>
+      <c r="N4" s="58">
+        <v>0.45168989992585939</v>
+      </c>
+      <c r="O4" s="58">
+        <v>0.42247144953337212</v>
+      </c>
+      <c r="P4" s="58">
+        <v>0.41177611120618529</v>
+      </c>
+      <c r="Q4" s="60">
+        <v>0.34946955395097867</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="63" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="57">
+        <v>1.0490137114163001</v>
+      </c>
+      <c r="D5" s="57">
+        <v>1.434982139485669</v>
+      </c>
+      <c r="E5" s="57">
+        <v>1.2943047991730501</v>
+      </c>
+      <c r="F5" s="57">
+        <v>1.2391795365528739</v>
+      </c>
+      <c r="G5" s="57">
+        <v>1.3694102876617571</v>
+      </c>
+      <c r="H5" s="57">
+        <v>1.443042284823141</v>
+      </c>
+      <c r="I5" s="57">
+        <v>1.3700343552736449</v>
+      </c>
+      <c r="J5" s="57">
+        <v>1.299822883627044</v>
+      </c>
+      <c r="K5" s="57">
+        <v>1.350071627379829</v>
+      </c>
+      <c r="L5" s="57">
+        <v>1.248677773165314</v>
+      </c>
+      <c r="M5" s="57">
+        <v>1.212098843731839</v>
+      </c>
+      <c r="N5" s="57">
+        <v>1.0981818670917001</v>
+      </c>
+      <c r="O5" s="57">
+        <v>1.0119847234027859</v>
+      </c>
+      <c r="P5" s="57">
+        <v>0.99890562562774432</v>
+      </c>
+      <c r="Q5" s="61">
+        <v>0.91153359502956166</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="62" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="58">
+        <v>-0.57544962133575761</v>
+      </c>
+      <c r="D6" s="58">
+        <v>-0.19549829188749829</v>
+      </c>
+      <c r="E6" s="58">
+        <v>-0.15163963681265219</v>
+      </c>
+      <c r="F6" s="58">
+        <v>-0.31019878694465541</v>
+      </c>
+      <c r="G6" s="58">
+        <v>-0.27765141209030197</v>
+      </c>
+      <c r="H6" s="58">
+        <v>-0.21299648359270409</v>
+      </c>
+      <c r="I6" s="58">
+        <v>-0.2098310782613807</v>
+      </c>
+      <c r="J6" s="58">
+        <v>-0.1932366748722153</v>
+      </c>
+      <c r="K6" s="58">
+        <v>-0.22183807121746441</v>
+      </c>
+      <c r="L6" s="58">
+        <v>-0.19275918118383559</v>
+      </c>
+      <c r="M6" s="58">
+        <v>-0.17331960112314251</v>
+      </c>
+      <c r="N6" s="58">
+        <v>-0.20620580112628589</v>
+      </c>
+      <c r="O6" s="58">
+        <v>-0.2046546717033354</v>
+      </c>
+      <c r="P6" s="58">
+        <v>-0.20626312632416219</v>
+      </c>
+      <c r="Q6" s="60">
+        <v>-0.23163087276473621</v>
+      </c>
+      <c r="S6" s="4"/>
+    </row>
+    <row r="7" spans="2:19" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="66" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="66"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="66"/>
+      <c r="H8" s="66"/>
+      <c r="I8" s="66"/>
+      <c r="J8" s="66"/>
+      <c r="K8" s="66"/>
+      <c r="L8" s="66"/>
+      <c r="M8" s="66"/>
+      <c r="N8" s="66"/>
+      <c r="O8" s="66"/>
+      <c r="P8" s="66"/>
+      <c r="Q8" s="66"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="B8:Q8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25C3ECDC-F20E-4773-9F8E-9FC7ED3C0073}">
   <dimension ref="A1:V32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2690,67 +2756,67 @@
       <c r="A2" s="1">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="4">
         <v>1.5333735802198469</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="5">
         <v>1.596869174740523</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="4">
         <v>1.582347559265874</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="4">
         <v>1.566947092709065</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="4">
         <v>1.530415912684481</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="4">
         <v>1.469854762322756</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="4">
         <v>1.4475112002117669</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="4">
         <v>1.484081000222448</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="4">
         <v>1.482282671066411</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="4">
         <v>1.4055404243803351</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="4">
         <v>1.310588101654018</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="4">
         <v>1.378627975958977</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="4">
         <v>1.3892558408758691</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="4">
         <v>1.3566022328377061</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="4">
         <v>1.295385014434373</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="4">
         <v>1.291870985256788</v>
       </c>
-      <c r="R2">
+      <c r="R2" s="4">
         <v>1.228204715093187</v>
       </c>
-      <c r="S2">
+      <c r="S2" s="4">
         <v>1.271579634166822</v>
       </c>
-      <c r="T2">
+      <c r="T2" s="4">
         <v>1.2379686823037901</v>
       </c>
-      <c r="U2">
+      <c r="U2" s="4">
         <v>1.20799724914692</v>
       </c>
-      <c r="V2">
+      <c r="V2" s="4">
         <v>1.1903486364110509</v>
       </c>
     </row>
@@ -2758,67 +2824,67 @@
       <c r="A3" s="1">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="4">
         <v>1.515480434613782</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="4">
         <v>1.5175694065755549</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="4">
         <v>1.4966573161455059</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="4">
         <v>1.503292107027653</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="4">
         <v>1.494735992530976</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="4">
         <v>1.4818505333396621</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="4">
         <v>1.5088451791428481</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="4">
         <v>1.403519631004589</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="4">
         <v>1.3923520778926319</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="4">
         <v>1.448145323454441</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="4">
         <v>1.4201500267555029</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="4">
         <v>1.3612117723483139</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="4">
         <v>1.3635377258326631</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="4">
         <v>1.338338073518357</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="4">
         <v>1.350372999192073</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="4">
         <v>1.314119735727747</v>
       </c>
-      <c r="R3">
+      <c r="R3" s="4">
         <v>1.277966870710229</v>
       </c>
-      <c r="S3">
+      <c r="S3" s="4">
         <v>1.25908161593089</v>
       </c>
-      <c r="T3">
+      <c r="T3" s="4">
         <v>1.1874703924113239</v>
       </c>
-      <c r="U3">
+      <c r="U3" s="4">
         <v>1.198730793654309</v>
       </c>
-      <c r="V3">
+      <c r="V3" s="4">
         <v>1.222139587123183</v>
       </c>
     </row>
@@ -2826,67 +2892,67 @@
       <c r="A4" s="1">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="4">
         <v>1.4559649431196451</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="4">
         <v>1.4307138698993891</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="4">
         <v>1.424147943635367</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="4">
         <v>1.458466803903091</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="4">
         <v>1.4648886562783969</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="4">
         <v>1.452233011875006</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="4">
         <v>1.4687495197239051</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="4">
         <v>1.446987549668566</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="4">
         <v>1.3406573665830781</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="4">
         <v>1.366738344814751</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="4">
         <v>1.3564831694799251</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="4">
         <v>1.3672783306330669</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="4">
         <v>1.379936347921874</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="4">
         <v>1.2855769815782629</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="4">
         <v>1.3082391548492089</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="4">
         <v>1.2755549494613421</v>
       </c>
-      <c r="R4">
+      <c r="R4" s="4">
         <v>1.287748658780324</v>
       </c>
-      <c r="S4">
+      <c r="S4" s="4">
         <v>1.190502377726429</v>
       </c>
-      <c r="T4">
+      <c r="T4" s="4">
         <v>1.21239622834178</v>
       </c>
-      <c r="U4">
+      <c r="U4" s="4">
         <v>1.206459392163777</v>
       </c>
-      <c r="V4">
+      <c r="V4" s="4">
         <v>1.2126433071410041</v>
       </c>
     </row>
@@ -2894,67 +2960,67 @@
       <c r="A5" s="1">
         <v>5</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="4">
         <v>1.4148776163061501</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="4">
         <v>1.3949858101629169</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="4">
         <v>1.407888016955996</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="4">
         <v>1.3866913348542069</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="4">
         <v>1.3765988987945901</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="4">
         <v>1.4021531352731329</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="4">
         <v>1.409742181502736</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="4">
         <v>1.3835132486074451</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="4">
         <v>1.3767105372936039</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="4">
         <v>1.306178658250936</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="4">
         <v>1.320903725539412</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="4">
         <v>1.309993147026238</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="4">
         <v>1.32725783573554</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="4">
         <v>1.29859947455727</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="4">
         <v>1.290934280306975</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="4">
         <v>1.2805472850423569</v>
       </c>
-      <c r="R5">
+      <c r="R5" s="4">
         <v>1.2543466900371421</v>
       </c>
-      <c r="S5">
+      <c r="S5" s="4">
         <v>1.2454438366699889</v>
       </c>
-      <c r="T5">
+      <c r="T5" s="4">
         <v>1.219236453667317</v>
       </c>
-      <c r="U5">
+      <c r="U5" s="4">
         <v>1.196638020302542</v>
       </c>
-      <c r="V5">
+      <c r="V5" s="4">
         <v>1.188275801869273</v>
       </c>
     </row>
@@ -2962,67 +3028,67 @@
       <c r="A6" s="1">
         <v>6</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="4">
         <v>1.398403295840509</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="4">
         <v>1.3884435809143481</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="4">
         <v>1.3997607257652021</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="4">
         <v>1.380030707932361</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="4">
         <v>1.4268588335684991</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="4">
         <v>1.3682371352152221</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="4">
         <v>1.3282097564529689</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="4">
         <v>1.3304640274451189</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="4">
         <v>1.3271038031415201</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="4">
         <v>1.2881167414201911</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="4">
         <v>1.26101103639281</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="4">
         <v>1.267875634133754</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="4">
         <v>1.328119915305104</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="4">
         <v>1.307101023609383</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="4">
         <v>1.309141500406749</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="4">
         <v>1.28107761876551</v>
       </c>
-      <c r="R6">
+      <c r="R6" s="4">
         <v>1.2745022370225529</v>
       </c>
-      <c r="S6">
+      <c r="S6" s="4">
         <v>1.254798714998705</v>
       </c>
-      <c r="T6">
+      <c r="T6" s="4">
         <v>1.2076641923439511</v>
       </c>
-      <c r="U6">
+      <c r="U6" s="4">
         <v>1.239385090378593</v>
       </c>
-      <c r="V6">
+      <c r="V6" s="4">
         <v>1.2239761362433981</v>
       </c>
     </row>
@@ -3030,67 +3096,67 @@
       <c r="A7" s="1">
         <v>7</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="4">
         <v>1.386214809257315</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="4">
         <v>1.4029831033721041</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="4">
         <v>1.417864609088251</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="4">
         <v>1.3733488858407941</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="4">
         <v>1.352632188054032</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="4">
         <v>1.323241694098785</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="4">
         <v>1.2990126735722041</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="4">
         <v>1.355232418796753</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="4">
         <v>1.3223570512240621</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="4">
         <v>1.285101218062435</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="4">
         <v>1.2885318893800819</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="4">
         <v>1.2729271950656611</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="4">
         <v>1.311293765810235</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="4">
         <v>1.271755981602402</v>
       </c>
-      <c r="P7">
+      <c r="P7" s="4">
         <v>1.2492332717163199</v>
       </c>
-      <c r="Q7">
+      <c r="Q7" s="4">
         <v>1.284861781658954</v>
       </c>
-      <c r="R7">
+      <c r="R7" s="4">
         <v>1.233197337769218</v>
       </c>
-      <c r="S7">
+      <c r="S7" s="4">
         <v>1.2328434433078641</v>
       </c>
-      <c r="T7">
+      <c r="T7" s="4">
         <v>1.2168240437215621</v>
       </c>
-      <c r="U7">
+      <c r="U7" s="4">
         <v>1.239029129157823</v>
       </c>
-      <c r="V7">
+      <c r="V7" s="4">
         <v>1.2345148773242749</v>
       </c>
     </row>
@@ -3098,67 +3164,67 @@
       <c r="A8" s="1">
         <v>8</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="4">
         <v>1.400727222190187</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="4">
         <v>1.4195528648463529</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="4">
         <v>1.3873817515533109</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="4">
         <v>1.3319604957485141</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="4">
         <v>1.3418092978563869</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="4">
         <v>1.3253472792673759</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="4">
         <v>1.2913957012028019</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="4">
         <v>1.324706041277159</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="4">
         <v>1.3357662401377111</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="4">
         <v>1.337733195595183</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="4">
         <v>1.293523258274383</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="4">
         <v>1.240892539006291</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="4">
         <v>1.2502758119998509</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="4">
         <v>1.222905079045205</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="4">
         <v>1.2142071468598901</v>
       </c>
-      <c r="Q8">
+      <c r="Q8" s="4">
         <v>1.1898922556881339</v>
       </c>
-      <c r="R8">
+      <c r="R8" s="4">
         <v>1.241754524379685</v>
       </c>
-      <c r="S8">
+      <c r="S8" s="4">
         <v>1.2353411282286679</v>
       </c>
-      <c r="T8">
+      <c r="T8" s="4">
         <v>1.2163304314498069</v>
       </c>
-      <c r="U8">
+      <c r="U8" s="4">
         <v>1.2258620041127619</v>
       </c>
-      <c r="V8">
+      <c r="V8" s="4">
         <v>1.190730903356781</v>
       </c>
     </row>
@@ -3166,67 +3232,67 @@
       <c r="A9" s="1">
         <v>9</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="4">
         <v>1.4136434738399459</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="4">
         <v>1.375046426407819</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="4">
         <v>1.3521428895805681</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="4">
         <v>1.336402748665438</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="4">
         <v>1.315674520166219</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="4">
         <v>1.3012459189972601</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="4">
         <v>1.2920412844684459</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="4">
         <v>1.308345942715218</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="4">
         <v>1.323199407364003</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="4">
         <v>1.2932087524807041</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="4">
         <v>1.2952742980529111</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="4">
         <v>1.2319028464462241</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="4">
         <v>1.2041182808605051</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="4">
         <v>1.2302335710761201</v>
       </c>
-      <c r="P9">
+      <c r="P9" s="4">
         <v>1.1890920602228161</v>
       </c>
-      <c r="Q9">
+      <c r="Q9" s="4">
         <v>1.223080482901129</v>
       </c>
-      <c r="R9">
+      <c r="R9" s="4">
         <v>1.2256282328441841</v>
       </c>
-      <c r="S9">
+      <c r="S9" s="4">
         <v>1.175816280018102</v>
       </c>
-      <c r="T9">
+      <c r="T9" s="4">
         <v>1.2252722494037489</v>
       </c>
-      <c r="U9">
+      <c r="U9" s="4">
         <v>1.2394441286504601</v>
       </c>
-      <c r="V9">
+      <c r="V9" s="4">
         <v>1.207060791281843</v>
       </c>
     </row>
@@ -3234,67 +3300,67 @@
       <c r="A10" s="1">
         <v>10</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="4">
         <v>1.3662043405627839</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="4">
         <v>1.3564123297726249</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="4">
         <v>1.3506785270883439</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="4">
         <v>1.3213144009913631</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="4">
         <v>1.303507256675829</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="4">
         <v>1.3065980353530811</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="4">
         <v>1.347073402364702</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="4">
         <v>1.3639909459510151</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="4">
         <v>1.337978570053975</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="4">
         <v>1.300116418323801</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="4">
         <v>1.245890941094292</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="4">
         <v>1.2304821167616471</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="4">
         <v>1.2238038709858809</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="4">
         <v>1.232720024742018</v>
       </c>
-      <c r="P10">
+      <c r="P10" s="4">
         <v>1.1848189244038649</v>
       </c>
-      <c r="Q10">
+      <c r="Q10" s="4">
         <v>1.21535519403638</v>
       </c>
-      <c r="R10">
+      <c r="R10" s="4">
         <v>1.182559156904903</v>
       </c>
-      <c r="S10">
+      <c r="S10" s="4">
         <v>1.1870853987215171</v>
       </c>
-      <c r="T10">
+      <c r="T10" s="4">
         <v>1.200912378208133</v>
       </c>
-      <c r="U10">
+      <c r="U10" s="4">
         <v>1.2114351128324741</v>
       </c>
-      <c r="V10">
+      <c r="V10" s="4">
         <v>1.1952535588510449</v>
       </c>
     </row>
@@ -4073,67 +4139,67 @@
       <c r="A24" s="1">
         <v>2</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="4">
         <v>-0.19153794297157309</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="4">
         <v>-0.19303313031771499</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="4">
         <v>-0.1753174072606577</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="4">
         <v>-0.18425905347408089</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="4">
         <v>-0.26387926527772892</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="4">
         <v>-0.247135038160821</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="4">
         <v>-0.28078357636022822</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="4">
         <v>-0.29765497169535771</v>
       </c>
-      <c r="J24">
+      <c r="J24" s="4">
         <v>-0.27689515624033978</v>
       </c>
-      <c r="K24">
+      <c r="K24" s="4">
         <v>-0.2666930168162735</v>
       </c>
-      <c r="L24">
+      <c r="L24" s="4">
         <v>-0.19624266600451901</v>
       </c>
-      <c r="M24">
+      <c r="M24" s="4">
         <v>-0.22999533613888579</v>
       </c>
-      <c r="N24">
+      <c r="N24" s="4">
         <v>-0.17348333145759751</v>
       </c>
-      <c r="O24">
+      <c r="O24" s="4">
         <v>-0.21951082478749689</v>
       </c>
-      <c r="P24">
+      <c r="P24" s="4">
         <v>-0.15743843457810991</v>
       </c>
-      <c r="Q24">
+      <c r="Q24" s="4">
         <v>-0.18516544242956079</v>
       </c>
-      <c r="R24">
+      <c r="R24" s="4">
         <v>-0.2109386361529591</v>
       </c>
-      <c r="S24">
+      <c r="S24" s="4">
         <v>-0.20160106425666419</v>
       </c>
-      <c r="T24">
+      <c r="T24" s="4">
         <v>-0.16908640956672011</v>
       </c>
-      <c r="U24">
+      <c r="U24" s="4">
         <v>-0.16461208146101919</v>
       </c>
-      <c r="V24">
+      <c r="V24" s="4">
         <v>-0.18007411681755051</v>
       </c>
     </row>
@@ -4141,67 +4207,67 @@
       <c r="A25" s="1">
         <v>3</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="4">
         <v>-0.24312871564870631</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="4">
         <v>-0.27113596305630971</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="4">
         <v>-0.16939417436033999</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="4">
         <v>-0.19432875514717271</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="4">
         <v>-0.23458982422096061</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="4">
         <v>-0.26308223589208329</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="4">
         <v>-0.26659688220408789</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="4">
         <v>-0.28938688360075648</v>
       </c>
-      <c r="J25">
+      <c r="J25" s="4">
         <v>-0.26432834320691972</v>
       </c>
-      <c r="K25">
+      <c r="K25" s="4">
         <v>-0.2170684490448111</v>
       </c>
-      <c r="L25">
+      <c r="L25" s="4">
         <v>-0.22499184877779921</v>
       </c>
-      <c r="M25">
+      <c r="M25" s="4">
         <v>-0.18653730591908299</v>
       </c>
-      <c r="N25">
+      <c r="N25" s="4">
         <v>-0.17126961812541591</v>
       </c>
-      <c r="O25">
+      <c r="O25" s="4">
         <v>-0.19240005593944021</v>
       </c>
-      <c r="P25">
+      <c r="P25" s="4">
         <v>-0.18765447640135899</v>
       </c>
-      <c r="Q25">
+      <c r="Q25" s="4">
         <v>-0.19961978133742461</v>
       </c>
-      <c r="R25">
+      <c r="R25" s="4">
         <v>-0.20508725050757329</v>
       </c>
-      <c r="S25">
+      <c r="S25" s="4">
         <v>-0.20772487551985269</v>
       </c>
-      <c r="T25">
+      <c r="T25" s="4">
         <v>-0.22480385781784271</v>
       </c>
-      <c r="U25">
+      <c r="U25" s="4">
         <v>-0.25179724928552571</v>
       </c>
-      <c r="V25">
+      <c r="V25" s="4">
         <v>-0.26357165784328851</v>
       </c>
     </row>
@@ -4209,67 +4275,67 @@
       <c r="A26" s="1">
         <v>4</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="4">
         <v>-0.2658367292267213</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="4">
         <v>-0.1873214889095392</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="5">
         <v>-0.1621286206620878</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="4">
         <v>-0.19268247868320379</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="4">
         <v>-0.1792389948632814</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="4">
         <v>-0.24291912857255801</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="4">
         <v>-0.26932716659790079</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="4">
         <v>-0.23231647196831201</v>
       </c>
-      <c r="J26">
+      <c r="J26" s="4">
         <v>-0.27981201620411578</v>
       </c>
-      <c r="K26">
+      <c r="K26" s="4">
         <v>-0.2201882864995178</v>
       </c>
-      <c r="L26">
+      <c r="L26" s="4">
         <v>-0.25167334127104768</v>
       </c>
-      <c r="M26">
+      <c r="M26" s="4">
         <v>-0.22130935222494891</v>
       </c>
-      <c r="N26">
+      <c r="N26" s="4">
         <v>-0.2213337067070088</v>
       </c>
-      <c r="O26">
+      <c r="O26" s="4">
         <v>-0.22076899836696701</v>
       </c>
-      <c r="P26">
+      <c r="P26" s="4">
         <v>-0.16527966328842991</v>
       </c>
-      <c r="Q26">
+      <c r="Q26" s="4">
         <v>-0.187498888316665</v>
       </c>
-      <c r="R26">
+      <c r="R26" s="4">
         <v>-0.20775696164107479</v>
       </c>
-      <c r="S26">
+      <c r="S26" s="4">
         <v>-0.2267339961631861</v>
       </c>
-      <c r="T26">
+      <c r="T26" s="4">
         <v>-0.25454961060979792</v>
       </c>
-      <c r="U26">
+      <c r="U26" s="4">
         <v>-0.27771594196044752</v>
       </c>
-      <c r="V26">
+      <c r="V26" s="4">
         <v>-0.26868529350546971</v>
       </c>
     </row>
@@ -4277,67 +4343,67 @@
       <c r="A27" s="1">
         <v>5</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="4">
         <v>-0.23024429772984251</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="4">
         <v>-0.16428958197406171</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="4">
         <v>-0.21138168051992301</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="4">
         <v>-0.24546215975811919</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="4">
         <v>-0.23104921302808731</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="4">
         <v>-0.24094139418984781</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="4">
         <v>-0.19608801093899481</v>
       </c>
-      <c r="I27">
+      <c r="I27" s="4">
         <v>-0.21996719882233279</v>
       </c>
-      <c r="J27">
+      <c r="J27" s="4">
         <v>-0.23638738183561189</v>
       </c>
-      <c r="K27">
+      <c r="K27" s="4">
         <v>-0.24375372627087971</v>
       </c>
-      <c r="L27">
+      <c r="L27" s="4">
         <v>-0.22444362767908699</v>
       </c>
-      <c r="M27">
+      <c r="M27" s="4">
         <v>-0.25853463036275792</v>
       </c>
-      <c r="N27">
+      <c r="N27" s="4">
         <v>-0.25749902519932488</v>
       </c>
-      <c r="O27">
+      <c r="O27" s="4">
         <v>-0.21957541868953651</v>
       </c>
-      <c r="P27">
+      <c r="P27" s="4">
         <v>-0.2026284597723581</v>
       </c>
-      <c r="Q27" s="2">
+      <c r="Q27" s="5">
         <v>-0.14277702074313231</v>
       </c>
-      <c r="R27">
+      <c r="R27" s="4">
         <v>-0.1839026140957693</v>
       </c>
-      <c r="S27">
+      <c r="S27" s="4">
         <v>-0.19572229738744051</v>
       </c>
-      <c r="T27">
+      <c r="T27" s="4">
         <v>-0.19318020744037551</v>
       </c>
-      <c r="U27">
+      <c r="U27" s="4">
         <v>-0.24720324394543111</v>
       </c>
-      <c r="V27">
+      <c r="V27" s="4">
         <v>-0.2408059394250468</v>
       </c>
     </row>
@@ -4345,67 +4411,67 @@
       <c r="A28" s="1">
         <v>6</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="4">
         <v>-0.20806155390924541</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="4">
         <v>-0.21135256460184659</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="4">
         <v>-0.25274679279645329</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="4">
         <v>-0.27673047935048889</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="4">
         <v>-0.24612804108083039</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="4">
         <v>-0.23602810521839951</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="4">
         <v>-0.26483923659976899</v>
       </c>
-      <c r="I28">
+      <c r="I28" s="4">
         <v>-0.2475230637621845</v>
       </c>
-      <c r="J28">
+      <c r="J28" s="4">
         <v>-0.2326176811983712</v>
       </c>
-      <c r="K28">
+      <c r="K28" s="4">
         <v>-0.26145166720780089</v>
       </c>
-      <c r="L28">
+      <c r="L28" s="4">
         <v>-0.28317589267612697</v>
       </c>
-      <c r="M28">
+      <c r="M28" s="4">
         <v>-0.27984235397637858</v>
       </c>
-      <c r="N28">
+      <c r="N28" s="4">
         <v>-0.25567458693818468</v>
       </c>
-      <c r="O28">
+      <c r="O28" s="4">
         <v>-0.2079987396407624</v>
       </c>
-      <c r="P28">
+      <c r="P28" s="4">
         <v>-0.18893146132806871</v>
       </c>
-      <c r="Q28">
+      <c r="Q28" s="4">
         <v>-0.16026881875122909</v>
       </c>
-      <c r="R28">
+      <c r="R28" s="4">
         <v>-0.1425600978488748</v>
       </c>
-      <c r="S28">
+      <c r="S28" s="4">
         <v>-0.1840386602028338</v>
       </c>
-      <c r="T28">
+      <c r="T28" s="4">
         <v>-0.20270090769564639</v>
       </c>
-      <c r="U28">
+      <c r="U28" s="4">
         <v>-0.23964371625644371</v>
       </c>
-      <c r="V28">
+      <c r="V28" s="4">
         <v>-0.21369578090810001</v>
       </c>
     </row>
@@ -4413,67 +4479,67 @@
       <c r="A29" s="1">
         <v>7</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="4">
         <v>-0.18397891864954441</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="4">
         <v>-0.21171509008698869</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="4">
         <v>-0.23795275314799569</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="4">
         <v>-0.27331738978689363</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="4">
         <v>-0.2411691701599534</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="4">
         <v>-0.27139040086218541</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="4">
         <v>-0.27980696642535691</v>
       </c>
-      <c r="I29">
+      <c r="I29" s="4">
         <v>-0.2600409491156237</v>
       </c>
-      <c r="J29">
+      <c r="J29" s="4">
         <v>-0.2579522978038129</v>
       </c>
-      <c r="K29">
+      <c r="K29" s="4">
         <v>-0.294133160376159</v>
       </c>
-      <c r="L29">
+      <c r="L29" s="4">
         <v>-0.25994452071766638</v>
       </c>
-      <c r="M29">
+      <c r="M29" s="4">
         <v>-0.26985080026397928</v>
       </c>
-      <c r="N29">
+      <c r="N29" s="4">
         <v>-0.28906868820983311</v>
       </c>
-      <c r="O29">
+      <c r="O29" s="4">
         <v>-0.24719124639184301</v>
       </c>
-      <c r="P29">
+      <c r="P29" s="4">
         <v>-0.18489136742910081</v>
       </c>
-      <c r="Q29">
+      <c r="Q29" s="4">
         <v>-0.16591182850974279</v>
       </c>
-      <c r="R29">
+      <c r="R29" s="4">
         <v>-0.15085262587762571</v>
       </c>
-      <c r="S29">
+      <c r="S29" s="4">
         <v>-0.16051146453062429</v>
       </c>
-      <c r="T29">
+      <c r="T29" s="4">
         <v>-0.16695475962027359</v>
       </c>
-      <c r="U29">
+      <c r="U29" s="4">
         <v>-0.20582568336585549</v>
       </c>
-      <c r="V29">
+      <c r="V29" s="4">
         <v>-0.18193622456181041</v>
       </c>
     </row>
@@ -4481,67 +4547,67 @@
       <c r="A30" s="1">
         <v>8</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="4">
         <v>-0.1997028966074243</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="4">
         <v>-0.22491458051828861</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="4">
         <v>-0.29908637446625458</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="4">
         <v>-0.26614722147059422</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="4">
         <v>-0.25495608667794178</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="4">
         <v>-0.23235784678386109</v>
       </c>
-      <c r="H30">
+      <c r="H30" s="4">
         <v>-0.26842879797147678</v>
       </c>
-      <c r="I30">
+      <c r="I30" s="4">
         <v>-0.26692762893622968</v>
       </c>
-      <c r="J30">
+      <c r="J30" s="4">
         <v>-0.2797619563885026</v>
       </c>
-      <c r="K30">
+      <c r="K30" s="4">
         <v>-0.25801398831778821</v>
       </c>
-      <c r="L30">
+      <c r="L30" s="4">
         <v>-0.2578382317477878</v>
       </c>
-      <c r="M30">
+      <c r="M30" s="4">
         <v>-0.2643275726587398</v>
       </c>
-      <c r="N30">
+      <c r="N30" s="4">
         <v>-0.26752691985271732</v>
       </c>
-      <c r="O30">
+      <c r="O30" s="4">
         <v>-0.25479531905100999</v>
       </c>
-      <c r="P30">
+      <c r="P30" s="4">
         <v>-0.19617414324726559</v>
       </c>
-      <c r="Q30">
+      <c r="Q30" s="4">
         <v>-0.16988924456087681</v>
       </c>
-      <c r="R30">
+      <c r="R30" s="4">
         <v>-0.15491361646987009</v>
       </c>
-      <c r="S30">
+      <c r="S30" s="4">
         <v>-0.17608422502277499</v>
       </c>
-      <c r="T30">
+      <c r="T30" s="4">
         <v>-0.18067932827242081</v>
       </c>
-      <c r="U30">
+      <c r="U30" s="4">
         <v>-0.19845633819330541</v>
       </c>
-      <c r="V30">
+      <c r="V30" s="4">
         <v>-0.19745223944941609</v>
       </c>
     </row>
@@ -4549,67 +4615,67 @@
       <c r="A31" s="1">
         <v>9</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="4">
         <v>-0.21989646549357059</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="4">
         <v>-0.27576822084574848</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="4">
         <v>-0.26554733218605281</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="4">
         <v>-0.25876103929104632</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="4">
         <v>-0.24439623352795861</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="4">
         <v>-0.25254986401125651</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="4">
         <v>-0.25636987861598742</v>
       </c>
-      <c r="I31">
+      <c r="I31" s="4">
         <v>-0.25792541964471699</v>
       </c>
-      <c r="J31">
+      <c r="J31" s="4">
         <v>-0.2813148955840038</v>
       </c>
-      <c r="K31">
+      <c r="K31" s="4">
         <v>-0.23980312913318341</v>
       </c>
-      <c r="L31">
+      <c r="L31" s="4">
         <v>-0.24307497121823249</v>
       </c>
-      <c r="M31">
+      <c r="M31" s="4">
         <v>-0.2173611294004919</v>
       </c>
-      <c r="N31">
+      <c r="N31" s="4">
         <v>-0.21483224285211769</v>
       </c>
-      <c r="O31">
+      <c r="O31" s="4">
         <v>-0.21246051194651541</v>
       </c>
-      <c r="P31">
+      <c r="P31" s="4">
         <v>-0.20381209965161159</v>
       </c>
-      <c r="Q31">
+      <c r="Q31" s="4">
         <v>-0.17909437754853169</v>
       </c>
-      <c r="R31">
+      <c r="R31" s="4">
         <v>-0.1852693235505386</v>
       </c>
-      <c r="S31">
+      <c r="S31" s="4">
         <v>-0.1751351963239377</v>
       </c>
-      <c r="T31">
+      <c r="T31" s="4">
         <v>-0.16392831271993399</v>
       </c>
-      <c r="U31">
+      <c r="U31" s="4">
         <v>-0.17756102629465359</v>
       </c>
-      <c r="V31">
+      <c r="V31" s="4">
         <v>-0.15849019722071889</v>
       </c>
     </row>
@@ -4617,67 +4683,67 @@
       <c r="A32" s="1">
         <v>10</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="4">
         <v>-0.27289785163205083</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="4">
         <v>-0.229422677068229</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="4">
         <v>-0.24870619489970311</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="4">
         <v>-0.2373076730118516</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="4">
         <v>-0.2315453212768748</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="4">
         <v>-0.24257899970576419</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="4">
         <v>-0.24647485781504611</v>
       </c>
-      <c r="I32">
+      <c r="I32" s="4">
         <v>-0.25879387093465323</v>
       </c>
-      <c r="J32">
+      <c r="J32" s="4">
         <v>-0.23891673676181091</v>
       </c>
-      <c r="K32">
+      <c r="K32" s="4">
         <v>-0.23122605374020039</v>
       </c>
-      <c r="L32">
+      <c r="L32" s="4">
         <v>-0.2193929054702933</v>
       </c>
-      <c r="M32">
+      <c r="M32" s="4">
         <v>-0.21698136605344509</v>
       </c>
-      <c r="N32">
+      <c r="N32" s="4">
         <v>-0.22114058807229431</v>
       </c>
-      <c r="O32">
+      <c r="O32" s="4">
         <v>-0.17572956083369279</v>
       </c>
-      <c r="P32">
+      <c r="P32" s="4">
         <v>-0.21590210485850961</v>
       </c>
-      <c r="Q32">
+      <c r="Q32" s="4">
         <v>-0.21922118686126821</v>
       </c>
-      <c r="R32">
+      <c r="R32" s="4">
         <v>-0.1863000875201197</v>
       </c>
-      <c r="S32">
+      <c r="S32" s="4">
         <v>-0.18727061913591039</v>
       </c>
-      <c r="T32">
+      <c r="T32" s="4">
         <v>-0.16920927679579109</v>
       </c>
-      <c r="U32">
+      <c r="U32" s="4">
         <v>-0.16405522907892209</v>
       </c>
-      <c r="V32">
+      <c r="V32" s="4">
         <v>-0.17355542706167301</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: final changes to spreadsheets
</commit_message>
<xml_diff>
--- a/results/robustness_checks_formatted.xlsx
+++ b/results/robustness_checks_formatted.xlsx
@@ -8,17 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\projects\python\bsic_systematic_fx\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94CDE65E-E4E6-416C-A7F1-6039CDA5B29F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DFAA5EC-320F-44C5-B951-0D2CD935C4A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="390" windowWidth="28800" windowHeight="15585" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1 (2)" sheetId="10" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="9" r:id="rId2"/>
+    <sheet name="final_fmt" sheetId="8" r:id="rId1"/>
+    <sheet name="paper_daily_rebalancing" sheetId="6" r:id="rId2"/>
     <sheet name="paper_weekly_rebalancing" sheetId="7" r:id="rId3"/>
-    <sheet name="paper" sheetId="6" r:id="rId4"/>
-    <sheet name="format_to_bsic_standards" sheetId="8" r:id="rId5"/>
-    <sheet name="improved_stats" sheetId="5" r:id="rId6"/>
+    <sheet name="paper_improved_daily_rebal" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,37 +35,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={4C33803E-CA15-40A6-9824-6737C0590958}</author>
-    <author>tc={9310CC52-D200-4E03-938E-C63E7AD85DF1}</author>
-  </authors>
-  <commentList>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{4C33803E-CA15-40A6-9824-6737C0590958}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Price @ 11/10: 0.313
-Fully Diluted Supply: 10,161,000,000</t>
-      </text>
-    </comment>
-    <comment ref="C4" authorId="1" shapeId="0" xr:uid="{9310CC52-D200-4E03-938E-C63E7AD85DF1}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Price @ 11/10: 2.2661
-Diluted Supply: 352,170,015</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>Total</t>
   </si>
@@ -81,88 +50,10 @@
     <t>average</t>
   </si>
   <si>
-    <t>Average</t>
-  </si>
-  <si>
     <t>2000-2010</t>
   </si>
   <si>
     <t>2010-2020</t>
-  </si>
-  <si>
-    <t>Key Financials (dollars in millions)</t>
-  </si>
-  <si>
-    <t>Centers</t>
-  </si>
-  <si>
-    <t>Total Patients</t>
-  </si>
-  <si>
-    <t>At-Risk</t>
-  </si>
-  <si>
-    <t>Fee-for-Service</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Revenues </t>
-  </si>
-  <si>
-    <t>$</t>
-  </si>
-  <si>
-    <t>Loss from Operations</t>
-  </si>
-  <si>
-    <t>Net Loss</t>
-  </si>
-  <si>
-    <t>Platform Contribution (Non-GAAP) (1)</t>
-  </si>
-  <si>
-    <t>Patient Contribution (Non-GAAP) (2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adjsuted EBITDA (Non-GAAP) (3) </t>
-  </si>
-  <si>
-    <t>(1) Defined as total revenues less the sum of medical claims expense and cost of care, excluding D&amp;A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(2) Defined as capitated revenue less medical claims expense </t>
-  </si>
-  <si>
-    <t>(3) Defined as net loss excluding interest expense and other income/ expense, income taxes, D&amp;A, transaction/offering related costs and stock and unit-based compensation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(2) Defined as total revenues less the sum of medical claims expense and cost of care, excluding depreciation and amortization </t>
-  </si>
-  <si>
-    <t>SOURCE: CoinMarketCap, FTX Balance Sheet from FT Article</t>
-  </si>
-  <si>
-    <t>% of fully diluted Mkt Cap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">as ratio of circulating Mkt Cap </t>
-  </si>
-  <si>
-    <t>FTX Holding Amount</t>
-  </si>
-  <si>
-    <t>Market Cap (Fully Diluted Supply)</t>
-  </si>
-  <si>
-    <t>Market Cap (Circulating Supply)</t>
-  </si>
-  <si>
-    <t>FTT</t>
-  </si>
-  <si>
-    <t>SRM</t>
-  </si>
-  <si>
-    <t>November 10, 2022 (USD, 000s)</t>
   </si>
   <si>
     <t>SR vs MA Window</t>
@@ -178,14 +69,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="#,##0;\(#,##0\)"/>
-    <numFmt numFmtId="165" formatCode="0.0%"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
+  <numFmts count="1">
     <numFmt numFmtId="167" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,13 +104,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Gill Sans MT"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Garamond"/>
@@ -245,50 +125,6 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Garamond"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Garamond"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Gill Sans MT"/>
@@ -302,7 +138,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -315,14 +151,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF002060"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="13">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -377,43 +207,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -463,11 +262,11 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -480,113 +279,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -609,65 +335,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>341358</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D32DD363-A7D8-46E5-A64B-945D8113F06C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7048500" y="2419350"/>
-          <a:ext cx="3708400" cy="1141458"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="ANDREA FRANCESCHINI" id="{0BF6F5A5-2E57-4713-B3C4-ABB599885732}" userId="S::andrea.franceschini2@studbocconi.it::14b07d3b-a333-49d2-a041-d4e0acdc572d" providerId="AD"/>
-</personList>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -955,387 +624,724 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="B4" dT="2022-11-23T15:40:11.80" personId="{0BF6F5A5-2E57-4713-B3C4-ABB599885732}" id="{4C33803E-CA15-40A6-9824-6737C0590958}">
-    <text>Price @ 11/10: 0.313
-Fully Diluted Supply: 10,161,000,000</text>
-  </threadedComment>
-  <threadedComment ref="C4" dT="2022-11-23T15:35:24.29" personId="{0BF6F5A5-2E57-4713-B3C4-ABB599885732}" id="{9310CC52-D200-4E03-938E-C63E7AD85DF1}">
-    <text>Price @ 11/10: 2.2661
-Diluted Supply: 352,170,015</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDB8F09B-C58C-4722-A195-25977BC66D5B}">
-  <dimension ref="A2:F9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5220731-67A1-4BB6-853C-66EAA50B4340}">
+  <dimension ref="B2:S8"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="109" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:Q8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" style="15" customWidth="1"/>
-    <col min="2" max="3" width="12.42578125" style="15" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" style="15"/>
-    <col min="5" max="5" width="13.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="12.5703125" style="15"/>
+    <col min="2" max="2" width="14.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="52" t="s">
+    <row r="2" spans="2:19" ht="16.5" x14ac:dyDescent="0.5">
+      <c r="B2" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+    </row>
+    <row r="3" spans="2:19" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="9">
+        <v>2</v>
+      </c>
+      <c r="D3" s="9">
+        <v>4</v>
+      </c>
+      <c r="E3" s="9">
+        <v>6</v>
+      </c>
+      <c r="F3" s="9">
+        <v>8</v>
+      </c>
+      <c r="G3" s="9">
+        <v>10</v>
+      </c>
+      <c r="H3" s="9">
+        <v>12</v>
+      </c>
+      <c r="I3" s="9">
+        <v>14</v>
+      </c>
+      <c r="J3" s="9">
+        <v>16</v>
+      </c>
+      <c r="K3" s="9">
+        <v>18</v>
+      </c>
+      <c r="L3" s="9">
+        <v>20</v>
+      </c>
+      <c r="M3" s="9">
+        <v>22</v>
+      </c>
+      <c r="N3" s="9">
+        <v>24</v>
+      </c>
+      <c r="O3" s="9">
+        <v>26</v>
+      </c>
+      <c r="P3" s="9">
+        <v>28</v>
+      </c>
+      <c r="Q3" s="10">
         <v>30</v>
       </c>
-      <c r="C2" s="51" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="50"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="48">
-        <v>82400</v>
-      </c>
-      <c r="C3" s="47">
-        <v>301440</v>
-      </c>
-      <c r="E3" s="49"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="48">
-        <v>3180393</v>
-      </c>
-      <c r="C4" s="47">
-        <v>798052.47099150007</v>
-      </c>
-      <c r="D4" s="46"/>
-    </row>
-    <row r="5" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="45">
-        <v>2187876.1719999998</v>
-      </c>
-      <c r="C5" s="44">
-        <v>553903.77300000004</v>
-      </c>
-      <c r="F5" s="43"/>
-    </row>
-    <row r="6" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="41">
-        <f>B$5/B3</f>
-        <v>26.551895291262134</v>
-      </c>
-      <c r="C6" s="40">
-        <f>C$5/C3</f>
-        <v>1.8375257862261147</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="39" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="38">
-        <f>B$5/B4</f>
-        <v>0.68792635752877074</v>
-      </c>
-      <c r="C7" s="37">
-        <f>C$5/C4</f>
-        <v>0.69406936653153928</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>23</v>
-      </c>
+    </row>
+    <row r="4" spans="2:19" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B4" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="12">
+        <v>0.10277109753760059</v>
+      </c>
+      <c r="D4" s="12">
+        <v>0.59300118816030833</v>
+      </c>
+      <c r="E4" s="12">
+        <v>0.57222594432367402</v>
+      </c>
+      <c r="F4" s="12">
+        <v>0.57086164296253339</v>
+      </c>
+      <c r="G4" s="13">
+        <v>0.64180904570128883</v>
+      </c>
+      <c r="H4" s="12">
+        <v>0.61085426480264182</v>
+      </c>
+      <c r="I4" s="12">
+        <v>0.57590467725145278</v>
+      </c>
+      <c r="J4" s="12">
+        <v>0.56236254763286742</v>
+      </c>
+      <c r="K4" s="12">
+        <v>0.57289810690953979</v>
+      </c>
+      <c r="L4" s="12">
+        <v>0.51874473895218609</v>
+      </c>
+      <c r="M4" s="12">
+        <v>0.50603392826946225</v>
+      </c>
+      <c r="N4" s="12">
+        <v>0.45168989992585939</v>
+      </c>
+      <c r="O4" s="12">
+        <v>0.42247144953337212</v>
+      </c>
+      <c r="P4" s="12">
+        <v>0.41177611120618529</v>
+      </c>
+      <c r="Q4" s="14">
+        <v>0.34946955395097867</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B5" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="11">
+        <v>1.0490137114163001</v>
+      </c>
+      <c r="D5" s="11">
+        <v>1.434982139485669</v>
+      </c>
+      <c r="E5" s="11">
+        <v>1.2943047991730501</v>
+      </c>
+      <c r="F5" s="11">
+        <v>1.2391795365528739</v>
+      </c>
+      <c r="G5" s="11">
+        <v>1.3694102876617571</v>
+      </c>
+      <c r="H5" s="11">
+        <v>1.443042284823141</v>
+      </c>
+      <c r="I5" s="11">
+        <v>1.3700343552736449</v>
+      </c>
+      <c r="J5" s="11">
+        <v>1.299822883627044</v>
+      </c>
+      <c r="K5" s="11">
+        <v>1.350071627379829</v>
+      </c>
+      <c r="L5" s="11">
+        <v>1.248677773165314</v>
+      </c>
+      <c r="M5" s="11">
+        <v>1.212098843731839</v>
+      </c>
+      <c r="N5" s="11">
+        <v>1.0981818670917001</v>
+      </c>
+      <c r="O5" s="11">
+        <v>1.0119847234027859</v>
+      </c>
+      <c r="P5" s="11">
+        <v>0.99890562562774432</v>
+      </c>
+      <c r="Q5" s="15">
+        <v>0.91153359502956166</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B6" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="12">
+        <v>-0.57544962133575761</v>
+      </c>
+      <c r="D6" s="12">
+        <v>-0.19549829188749829</v>
+      </c>
+      <c r="E6" s="12">
+        <v>-0.15163963681265219</v>
+      </c>
+      <c r="F6" s="12">
+        <v>-0.31019878694465541</v>
+      </c>
+      <c r="G6" s="12">
+        <v>-0.27765141209030197</v>
+      </c>
+      <c r="H6" s="12">
+        <v>-0.21299648359270409</v>
+      </c>
+      <c r="I6" s="12">
+        <v>-0.2098310782613807</v>
+      </c>
+      <c r="J6" s="12">
+        <v>-0.1932366748722153</v>
+      </c>
+      <c r="K6" s="12">
+        <v>-0.22183807121746441</v>
+      </c>
+      <c r="L6" s="12">
+        <v>-0.19275918118383559</v>
+      </c>
+      <c r="M6" s="12">
+        <v>-0.17331960112314251</v>
+      </c>
+      <c r="N6" s="12">
+        <v>-0.20620580112628589</v>
+      </c>
+      <c r="O6" s="12">
+        <v>-0.2046546717033354</v>
+      </c>
+      <c r="P6" s="12">
+        <v>-0.20626312632416219</v>
+      </c>
+      <c r="Q6" s="14">
+        <v>-0.23163087276473621</v>
+      </c>
+      <c r="S6" s="4"/>
+    </row>
+    <row r="7" spans="2:19" ht="7.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="2:19" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B8" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="19"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="B8:Q8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6089D506-DFB6-4A4A-ABA7-B4FAE6B969F1}">
-  <dimension ref="B2:F22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16E5077C-487C-40AA-9EB5-A098603EF849}">
+  <dimension ref="A1:U30"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="166" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:U4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="15"/>
-    <col min="2" max="2" width="37.85546875" style="15" customWidth="1"/>
-    <col min="3" max="3" width="5" style="15" customWidth="1"/>
-    <col min="4" max="16384" width="12.5703125" style="15"/>
+    <col min="6" max="6" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" s="11" customFormat="1" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B2" s="8" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>0.10277109753760059</v>
+      </c>
+      <c r="C2">
+        <v>1.0490137114163001</v>
+      </c>
+      <c r="D2">
+        <v>-0.57544962133575761</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>0.34160838310524672</v>
+      </c>
+      <c r="C3">
+        <v>1.2605139928505089</v>
+      </c>
+      <c r="D3">
+        <v>-0.36709689179061689</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>0.59300118816030833</v>
+      </c>
+      <c r="C4">
+        <v>1.434982139485669</v>
+      </c>
+      <c r="D4">
+        <v>-0.19549829188749829</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>0.60539159240027984</v>
+      </c>
+      <c r="C5">
+        <v>1.416075819373247</v>
+      </c>
+      <c r="D5">
+        <v>-0.2341401249189094</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>0.57222594432367402</v>
+      </c>
+      <c r="C6">
+        <v>1.2943047991730501</v>
+      </c>
+      <c r="D6" s="3">
+        <v>-0.15163963681265219</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
         <v>7</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9">
-        <v>2021</v>
-      </c>
-      <c r="E2" s="9">
-        <v>2020</v>
-      </c>
-      <c r="F2" s="10">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
+      <c r="B7">
+        <v>0.55842223206656061</v>
+      </c>
+      <c r="C7">
+        <v>1.2749858745559539</v>
+      </c>
+      <c r="D7">
+        <v>-0.21888069504539759</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
         <v>8</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13">
-        <v>129</v>
-      </c>
-      <c r="E3" s="13">
-        <v>79</v>
-      </c>
-      <c r="F3" s="14">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="18"/>
-    </row>
-    <row r="5" spans="2:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="19" t="s">
+      <c r="B8">
+        <v>0.57086164296253339</v>
+      </c>
+      <c r="C8">
+        <v>1.2391795365528739</v>
+      </c>
+      <c r="D8">
+        <v>-0.31019878694465541</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
         <v>9</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="21">
-        <v>153500</v>
-      </c>
-      <c r="E5" s="21">
-        <v>97000</v>
-      </c>
-      <c r="F5" s="22">
-        <v>79000</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="23" t="s">
+      <c r="B9" s="2">
+        <v>0.67201386179377598</v>
+      </c>
+      <c r="C9">
+        <v>1.421805507707574</v>
+      </c>
+      <c r="D9">
+        <v>-0.26334284893228838</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
         <v>10</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="25">
-        <v>114500</v>
-      </c>
-      <c r="E6" s="25">
-        <v>64500</v>
-      </c>
-      <c r="F6" s="26">
-        <v>48000</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="27" t="s">
+      <c r="B10">
+        <v>0.64180904570128883</v>
+      </c>
+      <c r="C10">
+        <v>1.3694102876617571</v>
+      </c>
+      <c r="D10">
+        <v>-0.27765141209030197</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
         <v>11</v>
       </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="29">
-        <v>39000</v>
-      </c>
-      <c r="E7" s="29">
-        <v>32500</v>
-      </c>
-      <c r="F7" s="30">
-        <v>31000</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="16"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="26"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="16" t="s">
+      <c r="B11">
+        <v>0.57032736557947727</v>
+      </c>
+      <c r="C11">
+        <v>1.377990398126913</v>
+      </c>
+      <c r="D11">
+        <v>-0.31379994175872522</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
         <v>12</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="B12">
+        <v>0.61085426480264182</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1.443042284823141</v>
+      </c>
+      <c r="D12">
+        <v>-0.21299648359270409</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
         <v>13</v>
       </c>
-      <c r="D9" s="25">
-        <v>1432.6</v>
-      </c>
-      <c r="E9" s="25">
-        <v>882.8</v>
-      </c>
-      <c r="F9" s="26">
-        <v>556.6</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="16" t="s">
+      <c r="B13">
+        <v>0.5554977578552931</v>
+      </c>
+      <c r="C13">
+        <v>1.3366347993427079</v>
+      </c>
+      <c r="D13">
+        <v>-0.25065401470962489</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
         <v>14</v>
       </c>
-      <c r="C10" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="25">
-        <v>-414</v>
-      </c>
-      <c r="E10" s="25">
-        <v>-183.5</v>
-      </c>
-      <c r="F10" s="26">
-        <v>-103.9</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="12" t="s">
+      <c r="B14">
+        <v>0.57590467725145278</v>
+      </c>
+      <c r="C14">
+        <v>1.3700343552736449</v>
+      </c>
+      <c r="D14">
+        <v>-0.2098310782613807</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
         <v>15</v>
       </c>
-      <c r="C11" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="29">
-        <v>-414.6</v>
-      </c>
-      <c r="E11" s="29">
-        <v>-192.1</v>
-      </c>
-      <c r="F11" s="30">
-        <v>-109.5</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="16"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="26"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="16" t="s">
+      <c r="B15">
+        <v>0.54483021543070509</v>
+      </c>
+      <c r="C15">
+        <v>1.304847941721532</v>
+      </c>
+      <c r="D15">
+        <v>-0.2392315726639995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
         <v>16</v>
       </c>
-      <c r="C13" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="25">
-        <v>31.5</v>
-      </c>
-      <c r="E13" s="25">
-        <v>77.5</v>
-      </c>
-      <c r="F13" s="26">
-        <v>29.7</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="16" t="s">
+      <c r="B16">
+        <v>0.56236254763286742</v>
+      </c>
+      <c r="C16">
+        <v>1.299822883627044</v>
+      </c>
+      <c r="D16">
+        <v>-0.1932366748722153</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
         <v>17</v>
       </c>
-      <c r="C14" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="25">
-        <v>288</v>
-      </c>
-      <c r="E14" s="25">
-        <v>233.5</v>
-      </c>
-      <c r="F14" s="26">
-        <v>153.9</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="12" t="s">
+      <c r="B17">
+        <v>0.53678454882109594</v>
+      </c>
+      <c r="C17">
+        <v>1.2632104455238251</v>
+      </c>
+      <c r="D17">
+        <v>-0.2206758743870027</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
         <v>18</v>
       </c>
-      <c r="C15" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="29">
-        <v>-228.9</v>
-      </c>
-      <c r="E15" s="29">
-        <v>-92.6</v>
-      </c>
-      <c r="F15" s="30">
-        <v>-88.3</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="64" t="s">
+      <c r="B18">
+        <v>0.57289810690953979</v>
+      </c>
+      <c r="C18">
+        <v>1.350071627379829</v>
+      </c>
+      <c r="D18">
+        <v>-0.22183807121746441</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
         <v>19</v>
       </c>
-      <c r="C16" s="64"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="64"/>
-      <c r="F16" s="64"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="64" t="s">
+      <c r="B19">
+        <v>0.50925843311604047</v>
+      </c>
+      <c r="C19">
+        <v>1.266678569887749</v>
+      </c>
+      <c r="D19">
+        <v>-0.22676741744922141</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
         <v>20</v>
       </c>
-      <c r="C17" s="64"/>
-      <c r="D17" s="64"/>
-      <c r="E17" s="64"/>
-      <c r="F17" s="64"/>
-    </row>
-    <row r="18" spans="2:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="64" t="s">
+      <c r="B20">
+        <v>0.51874473895218609</v>
+      </c>
+      <c r="C20">
+        <v>1.248677773165314</v>
+      </c>
+      <c r="D20">
+        <v>-0.19275918118383559</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
         <v>21</v>
       </c>
-      <c r="C18" s="64"/>
-      <c r="D18" s="64"/>
-      <c r="E18" s="64"/>
-      <c r="F18" s="64"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="35" t="s">
+      <c r="B21">
+        <v>0.51105749821954072</v>
+      </c>
+      <c r="C21">
+        <v>1.2440585308707359</v>
+      </c>
+      <c r="D21">
+        <v>-0.2374526082663018</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="35" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="35" t="s">
-        <v>21</v>
+      <c r="B22">
+        <v>0.50603392826946225</v>
+      </c>
+      <c r="C22">
+        <v>1.212098843731839</v>
+      </c>
+      <c r="D22">
+        <v>-0.17331960112314251</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>0.47054522344078481</v>
+      </c>
+      <c r="C23">
+        <v>1.169151838023373</v>
+      </c>
+      <c r="D23">
+        <v>-0.217066720707174</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="1">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>0.45168989992585939</v>
+      </c>
+      <c r="C24">
+        <v>1.0981818670917001</v>
+      </c>
+      <c r="D24">
+        <v>-0.20620580112628589</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>0.43367162594011632</v>
+      </c>
+      <c r="C25">
+        <v>1.033755214227813</v>
+      </c>
+      <c r="D25">
+        <v>-0.20374722085138081</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
+        <v>26</v>
+      </c>
+      <c r="B26">
+        <v>0.42247144953337212</v>
+      </c>
+      <c r="C26">
+        <v>1.0119847234027859</v>
+      </c>
+      <c r="D26">
+        <v>-0.2046546717033354</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="1">
+        <v>27</v>
+      </c>
+      <c r="B27">
+        <v>0.40438218341986942</v>
+      </c>
+      <c r="C27">
+        <v>0.98354190716406309</v>
+      </c>
+      <c r="D27">
+        <v>-0.21498258496046099</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="1">
+        <v>28</v>
+      </c>
+      <c r="B28">
+        <v>0.41177611120618529</v>
+      </c>
+      <c r="C28">
+        <v>0.99890562562774432</v>
+      </c>
+      <c r="D28">
+        <v>-0.20626312632416219</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="1">
+        <v>29</v>
+      </c>
+      <c r="B29">
+        <v>0.36005439656036881</v>
+      </c>
+      <c r="C29">
+        <v>0.93164666422371178</v>
+      </c>
+      <c r="D29">
+        <v>-0.27086756502918058</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="1">
+        <v>30</v>
+      </c>
+      <c r="B30">
+        <v>0.34946955395097867</v>
+      </c>
+      <c r="C30">
+        <v>0.91153359502956166</v>
+      </c>
+      <c r="D30">
+        <v>-0.23163087276473621</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1347,9 +1353,9 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1360,7 +1366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -1374,7 +1380,7 @@
         <v>-0.20249410649828309</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>3</v>
       </c>
@@ -1388,7 +1394,7 @@
         <v>-7.876662557922641E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>4</v>
       </c>
@@ -1402,7 +1408,7 @@
         <v>-0.16065664756425649</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>5</v>
       </c>
@@ -1416,7 +1422,7 @@
         <v>-0.1267082167877851</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>6</v>
       </c>
@@ -1430,7 +1436,7 @@
         <v>-0.16403832399525481</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>7</v>
       </c>
@@ -1444,7 +1450,7 @@
         <v>-0.1490302751699733</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>8</v>
       </c>
@@ -1458,7 +1464,7 @@
         <v>-0.1480636800199582</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>9</v>
       </c>
@@ -1472,7 +1478,7 @@
         <v>-0.116486713723608</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>10</v>
       </c>
@@ -1486,7 +1492,7 @@
         <v>-9.7318655691187375E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>11</v>
       </c>
@@ -1500,7 +1506,7 @@
         <v>-0.15126543298733669</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>12</v>
       </c>
@@ -1514,7 +1520,7 @@
         <v>-0.14359458729320879</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>13</v>
       </c>
@@ -1528,7 +1534,7 @@
         <v>-0.13453651610862299</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>14</v>
       </c>
@@ -1542,7 +1548,7 @@
         <v>-0.1208188658266121</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>15</v>
       </c>
@@ -1556,7 +1562,7 @@
         <v>-0.12725271128275159</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>16</v>
       </c>
@@ -1570,7 +1576,7 @@
         <v>-9.8739457005351999E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>17</v>
       </c>
@@ -1584,7 +1590,7 @@
         <v>-0.1121659427412897</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>18</v>
       </c>
@@ -1598,7 +1604,7 @@
         <v>-8.53382147817391E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>19</v>
       </c>
@@ -1612,7 +1618,7 @@
         <v>-0.12634624944370179</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>20</v>
       </c>
@@ -1626,7 +1632,7 @@
         <v>-0.1034439302258726</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>21</v>
       </c>
@@ -1640,7 +1646,7 @@
         <v>-0.1231374060553784</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>22</v>
       </c>
@@ -1654,7 +1660,7 @@
         <v>-8.9770842638382739E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>23</v>
       </c>
@@ -1668,7 +1674,7 @@
         <v>-0.12646349669098919</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>24</v>
       </c>
@@ -1682,7 +1688,7 @@
         <v>-9.9250419842135881E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>25</v>
       </c>
@@ -1696,7 +1702,7 @@
         <v>-0.1437366607378828</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>26</v>
       </c>
@@ -1710,7 +1716,7 @@
         <v>-0.11697001154882219</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>27</v>
       </c>
@@ -1724,7 +1730,7 @@
         <v>-0.1214222504464782</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>28</v>
       </c>
@@ -1738,7 +1744,7 @@
         <v>-0.13466841425919759</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>29</v>
       </c>
@@ -1752,7 +1758,7 @@
         <v>-0.1790283573912882</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>30</v>
       </c>
@@ -1766,7 +1772,7 @@
         <v>-0.2238306920591559</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B31">
         <f>MAX(B2:B30)</f>
         <v>0.2494283102632181</v>
@@ -1786,905 +1792,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16E5077C-487C-40AA-9EB5-A098603EF849}">
-  <dimension ref="A1:U30"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:U4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1">
-        <v>2</v>
-      </c>
-      <c r="H1" s="1">
-        <v>4</v>
-      </c>
-      <c r="I1" s="1">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1">
-        <v>12</v>
-      </c>
-      <c r="M1" s="1">
-        <v>14</v>
-      </c>
-      <c r="N1" s="1">
-        <v>16</v>
-      </c>
-      <c r="O1" s="1">
-        <v>18</v>
-      </c>
-      <c r="P1" s="1">
-        <v>20</v>
-      </c>
-      <c r="Q1" s="1">
-        <v>22</v>
-      </c>
-      <c r="R1" s="1">
-        <v>24</v>
-      </c>
-      <c r="S1" s="1">
-        <v>26</v>
-      </c>
-      <c r="T1" s="1">
-        <v>28</v>
-      </c>
-      <c r="U1" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>0.10277109753760059</v>
-      </c>
-      <c r="C2">
-        <v>1.0490137114163001</v>
-      </c>
-      <c r="D2">
-        <v>-0.57544962133575761</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2">
-        <v>0.10277109753760059</v>
-      </c>
-      <c r="H2">
-        <v>0.59300118816030833</v>
-      </c>
-      <c r="I2">
-        <v>0.57222594432367402</v>
-      </c>
-      <c r="J2">
-        <v>0.57086164296253339</v>
-      </c>
-      <c r="K2" s="3">
-        <v>0.64180904570128883</v>
-      </c>
-      <c r="L2">
-        <v>0.61085426480264182</v>
-      </c>
-      <c r="M2">
-        <v>0.57590467725145278</v>
-      </c>
-      <c r="N2">
-        <v>0.56236254763286742</v>
-      </c>
-      <c r="O2">
-        <v>0.57289810690953979</v>
-      </c>
-      <c r="P2">
-        <v>0.51874473895218609</v>
-      </c>
-      <c r="Q2">
-        <v>0.50603392826946225</v>
-      </c>
-      <c r="R2">
-        <v>0.45168989992585939</v>
-      </c>
-      <c r="S2">
-        <v>0.42247144953337212</v>
-      </c>
-      <c r="T2">
-        <v>0.41177611120618529</v>
-      </c>
-      <c r="U2">
-        <v>0.34946955395097867</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>0.34160838310524672</v>
-      </c>
-      <c r="C3">
-        <v>1.2605139928505089</v>
-      </c>
-      <c r="D3">
-        <v>-0.36709689179061689</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3">
-        <v>1.0490137114163001</v>
-      </c>
-      <c r="H3">
-        <v>1.434982139485669</v>
-      </c>
-      <c r="I3">
-        <v>1.2943047991730501</v>
-      </c>
-      <c r="J3">
-        <v>1.2391795365528739</v>
-      </c>
-      <c r="K3">
-        <v>1.3694102876617571</v>
-      </c>
-      <c r="L3" s="3">
-        <v>1.443042284823141</v>
-      </c>
-      <c r="M3">
-        <v>1.3700343552736449</v>
-      </c>
-      <c r="N3">
-        <v>1.299822883627044</v>
-      </c>
-      <c r="O3">
-        <v>1.350071627379829</v>
-      </c>
-      <c r="P3">
-        <v>1.248677773165314</v>
-      </c>
-      <c r="Q3">
-        <v>1.212098843731839</v>
-      </c>
-      <c r="R3">
-        <v>1.0981818670917001</v>
-      </c>
-      <c r="S3">
-        <v>1.0119847234027859</v>
-      </c>
-      <c r="T3">
-        <v>0.99890562562774432</v>
-      </c>
-      <c r="U3">
-        <v>0.91153359502956166</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>0.59300118816030833</v>
-      </c>
-      <c r="C4">
-        <v>1.434982139485669</v>
-      </c>
-      <c r="D4">
-        <v>-0.19549829188749829</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4">
-        <v>-0.57544962133575761</v>
-      </c>
-      <c r="H4">
-        <v>-0.19549829188749829</v>
-      </c>
-      <c r="I4" s="3">
-        <v>-0.15163963681265219</v>
-      </c>
-      <c r="J4">
-        <v>-0.31019878694465541</v>
-      </c>
-      <c r="K4">
-        <v>-0.27765141209030197</v>
-      </c>
-      <c r="L4">
-        <v>-0.21299648359270409</v>
-      </c>
-      <c r="M4">
-        <v>-0.2098310782613807</v>
-      </c>
-      <c r="N4">
-        <v>-0.1932366748722153</v>
-      </c>
-      <c r="O4">
-        <v>-0.22183807121746441</v>
-      </c>
-      <c r="P4">
-        <v>-0.19275918118383559</v>
-      </c>
-      <c r="Q4">
-        <v>-0.17331960112314251</v>
-      </c>
-      <c r="R4">
-        <v>-0.20620580112628589</v>
-      </c>
-      <c r="S4">
-        <v>-0.2046546717033354</v>
-      </c>
-      <c r="T4">
-        <v>-0.20626312632416219</v>
-      </c>
-      <c r="U4">
-        <v>-0.23163087276473621</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>0.60539159240027984</v>
-      </c>
-      <c r="C5">
-        <v>1.416075819373247</v>
-      </c>
-      <c r="D5">
-        <v>-0.2341401249189094</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>0.57222594432367402</v>
-      </c>
-      <c r="C6">
-        <v>1.2943047991730501</v>
-      </c>
-      <c r="D6" s="3">
-        <v>-0.15163963681265219</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>0.55842223206656061</v>
-      </c>
-      <c r="C7">
-        <v>1.2749858745559539</v>
-      </c>
-      <c r="D7">
-        <v>-0.21888069504539759</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>0.57086164296253339</v>
-      </c>
-      <c r="C8">
-        <v>1.2391795365528739</v>
-      </c>
-      <c r="D8">
-        <v>-0.31019878694465541</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>9</v>
-      </c>
-      <c r="B9" s="2">
-        <v>0.67201386179377598</v>
-      </c>
-      <c r="C9">
-        <v>1.421805507707574</v>
-      </c>
-      <c r="D9">
-        <v>-0.26334284893228838</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>10</v>
-      </c>
-      <c r="B10">
-        <v>0.64180904570128883</v>
-      </c>
-      <c r="C10">
-        <v>1.3694102876617571</v>
-      </c>
-      <c r="D10">
-        <v>-0.27765141209030197</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>11</v>
-      </c>
-      <c r="B11">
-        <v>0.57032736557947727</v>
-      </c>
-      <c r="C11">
-        <v>1.377990398126913</v>
-      </c>
-      <c r="D11">
-        <v>-0.31379994175872522</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>12</v>
-      </c>
-      <c r="B12">
-        <v>0.61085426480264182</v>
-      </c>
-      <c r="C12" s="3">
-        <v>1.443042284823141</v>
-      </c>
-      <c r="D12">
-        <v>-0.21299648359270409</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>13</v>
-      </c>
-      <c r="B13">
-        <v>0.5554977578552931</v>
-      </c>
-      <c r="C13">
-        <v>1.3366347993427079</v>
-      </c>
-      <c r="D13">
-        <v>-0.25065401470962489</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>14</v>
-      </c>
-      <c r="B14">
-        <v>0.57590467725145278</v>
-      </c>
-      <c r="C14">
-        <v>1.3700343552736449</v>
-      </c>
-      <c r="D14">
-        <v>-0.2098310782613807</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>15</v>
-      </c>
-      <c r="B15">
-        <v>0.54483021543070509</v>
-      </c>
-      <c r="C15">
-        <v>1.304847941721532</v>
-      </c>
-      <c r="D15">
-        <v>-0.2392315726639995</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>16</v>
-      </c>
-      <c r="B16">
-        <v>0.56236254763286742</v>
-      </c>
-      <c r="C16">
-        <v>1.299822883627044</v>
-      </c>
-      <c r="D16">
-        <v>-0.1932366748722153</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>17</v>
-      </c>
-      <c r="B17">
-        <v>0.53678454882109594</v>
-      </c>
-      <c r="C17">
-        <v>1.2632104455238251</v>
-      </c>
-      <c r="D17">
-        <v>-0.2206758743870027</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>18</v>
-      </c>
-      <c r="B18">
-        <v>0.57289810690953979</v>
-      </c>
-      <c r="C18">
-        <v>1.350071627379829</v>
-      </c>
-      <c r="D18">
-        <v>-0.22183807121746441</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>19</v>
-      </c>
-      <c r="B19">
-        <v>0.50925843311604047</v>
-      </c>
-      <c r="C19">
-        <v>1.266678569887749</v>
-      </c>
-      <c r="D19">
-        <v>-0.22676741744922141</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>20</v>
-      </c>
-      <c r="B20">
-        <v>0.51874473895218609</v>
-      </c>
-      <c r="C20">
-        <v>1.248677773165314</v>
-      </c>
-      <c r="D20">
-        <v>-0.19275918118383559</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>21</v>
-      </c>
-      <c r="B21">
-        <v>0.51105749821954072</v>
-      </c>
-      <c r="C21">
-        <v>1.2440585308707359</v>
-      </c>
-      <c r="D21">
-        <v>-0.2374526082663018</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>22</v>
-      </c>
-      <c r="B22">
-        <v>0.50603392826946225</v>
-      </c>
-      <c r="C22">
-        <v>1.212098843731839</v>
-      </c>
-      <c r="D22">
-        <v>-0.17331960112314251</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>23</v>
-      </c>
-      <c r="B23">
-        <v>0.47054522344078481</v>
-      </c>
-      <c r="C23">
-        <v>1.169151838023373</v>
-      </c>
-      <c r="D23">
-        <v>-0.217066720707174</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>24</v>
-      </c>
-      <c r="B24">
-        <v>0.45168989992585939</v>
-      </c>
-      <c r="C24">
-        <v>1.0981818670917001</v>
-      </c>
-      <c r="D24">
-        <v>-0.20620580112628589</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>25</v>
-      </c>
-      <c r="B25">
-        <v>0.43367162594011632</v>
-      </c>
-      <c r="C25">
-        <v>1.033755214227813</v>
-      </c>
-      <c r="D25">
-        <v>-0.20374722085138081</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>26</v>
-      </c>
-      <c r="B26">
-        <v>0.42247144953337212</v>
-      </c>
-      <c r="C26">
-        <v>1.0119847234027859</v>
-      </c>
-      <c r="D26">
-        <v>-0.2046546717033354</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>27</v>
-      </c>
-      <c r="B27">
-        <v>0.40438218341986942</v>
-      </c>
-      <c r="C27">
-        <v>0.98354190716406309</v>
-      </c>
-      <c r="D27">
-        <v>-0.21498258496046099</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>28</v>
-      </c>
-      <c r="B28">
-        <v>0.41177611120618529</v>
-      </c>
-      <c r="C28">
-        <v>0.99890562562774432</v>
-      </c>
-      <c r="D28">
-        <v>-0.20626312632416219</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>29</v>
-      </c>
-      <c r="B29">
-        <v>0.36005439656036881</v>
-      </c>
-      <c r="C29">
-        <v>0.93164666422371178</v>
-      </c>
-      <c r="D29">
-        <v>-0.27086756502918058</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>30</v>
-      </c>
-      <c r="B30">
-        <v>0.34946955395097867</v>
-      </c>
-      <c r="C30">
-        <v>0.91153359502956166</v>
-      </c>
-      <c r="D30">
-        <v>-0.23163087276473621</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5220731-67A1-4BB6-853C-66EAA50B4340}">
-  <dimension ref="B2:S8"/>
-  <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:Q8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:19" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="B2" s="65" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="65"/>
-      <c r="N2" s="65"/>
-      <c r="O2" s="65"/>
-      <c r="P2" s="65"/>
-      <c r="Q2" s="65"/>
-    </row>
-    <row r="3" spans="2:19" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="54" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="55">
-        <v>2</v>
-      </c>
-      <c r="D3" s="55">
-        <v>4</v>
-      </c>
-      <c r="E3" s="55">
-        <v>6</v>
-      </c>
-      <c r="F3" s="55">
-        <v>8</v>
-      </c>
-      <c r="G3" s="55">
-        <v>10</v>
-      </c>
-      <c r="H3" s="55">
-        <v>12</v>
-      </c>
-      <c r="I3" s="55">
-        <v>14</v>
-      </c>
-      <c r="J3" s="55">
-        <v>16</v>
-      </c>
-      <c r="K3" s="55">
-        <v>18</v>
-      </c>
-      <c r="L3" s="55">
-        <v>20</v>
-      </c>
-      <c r="M3" s="55">
-        <v>22</v>
-      </c>
-      <c r="N3" s="55">
-        <v>24</v>
-      </c>
-      <c r="O3" s="55">
-        <v>26</v>
-      </c>
-      <c r="P3" s="55">
-        <v>28</v>
-      </c>
-      <c r="Q3" s="56">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="62" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="58">
-        <v>0.10277109753760059</v>
-      </c>
-      <c r="D4" s="58">
-        <v>0.59300118816030833</v>
-      </c>
-      <c r="E4" s="58">
-        <v>0.57222594432367402</v>
-      </c>
-      <c r="F4" s="58">
-        <v>0.57086164296253339</v>
-      </c>
-      <c r="G4" s="59">
-        <v>0.64180904570128883</v>
-      </c>
-      <c r="H4" s="58">
-        <v>0.61085426480264182</v>
-      </c>
-      <c r="I4" s="58">
-        <v>0.57590467725145278</v>
-      </c>
-      <c r="J4" s="58">
-        <v>0.56236254763286742</v>
-      </c>
-      <c r="K4" s="58">
-        <v>0.57289810690953979</v>
-      </c>
-      <c r="L4" s="58">
-        <v>0.51874473895218609</v>
-      </c>
-      <c r="M4" s="58">
-        <v>0.50603392826946225</v>
-      </c>
-      <c r="N4" s="58">
-        <v>0.45168989992585939</v>
-      </c>
-      <c r="O4" s="58">
-        <v>0.42247144953337212</v>
-      </c>
-      <c r="P4" s="58">
-        <v>0.41177611120618529</v>
-      </c>
-      <c r="Q4" s="60">
-        <v>0.34946955395097867</v>
-      </c>
-    </row>
-    <row r="5" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="63" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="57">
-        <v>1.0490137114163001</v>
-      </c>
-      <c r="D5" s="57">
-        <v>1.434982139485669</v>
-      </c>
-      <c r="E5" s="57">
-        <v>1.2943047991730501</v>
-      </c>
-      <c r="F5" s="57">
-        <v>1.2391795365528739</v>
-      </c>
-      <c r="G5" s="57">
-        <v>1.3694102876617571</v>
-      </c>
-      <c r="H5" s="57">
-        <v>1.443042284823141</v>
-      </c>
-      <c r="I5" s="57">
-        <v>1.3700343552736449</v>
-      </c>
-      <c r="J5" s="57">
-        <v>1.299822883627044</v>
-      </c>
-      <c r="K5" s="57">
-        <v>1.350071627379829</v>
-      </c>
-      <c r="L5" s="57">
-        <v>1.248677773165314</v>
-      </c>
-      <c r="M5" s="57">
-        <v>1.212098843731839</v>
-      </c>
-      <c r="N5" s="57">
-        <v>1.0981818670917001</v>
-      </c>
-      <c r="O5" s="57">
-        <v>1.0119847234027859</v>
-      </c>
-      <c r="P5" s="57">
-        <v>0.99890562562774432</v>
-      </c>
-      <c r="Q5" s="61">
-        <v>0.91153359502956166</v>
-      </c>
-    </row>
-    <row r="6" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="62" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="58">
-        <v>-0.57544962133575761</v>
-      </c>
-      <c r="D6" s="58">
-        <v>-0.19549829188749829</v>
-      </c>
-      <c r="E6" s="58">
-        <v>-0.15163963681265219</v>
-      </c>
-      <c r="F6" s="58">
-        <v>-0.31019878694465541</v>
-      </c>
-      <c r="G6" s="58">
-        <v>-0.27765141209030197</v>
-      </c>
-      <c r="H6" s="58">
-        <v>-0.21299648359270409</v>
-      </c>
-      <c r="I6" s="58">
-        <v>-0.2098310782613807</v>
-      </c>
-      <c r="J6" s="58">
-        <v>-0.1932366748722153</v>
-      </c>
-      <c r="K6" s="58">
-        <v>-0.22183807121746441</v>
-      </c>
-      <c r="L6" s="58">
-        <v>-0.19275918118383559</v>
-      </c>
-      <c r="M6" s="58">
-        <v>-0.17331960112314251</v>
-      </c>
-      <c r="N6" s="58">
-        <v>-0.20620580112628589</v>
-      </c>
-      <c r="O6" s="58">
-        <v>-0.2046546717033354</v>
-      </c>
-      <c r="P6" s="58">
-        <v>-0.20626312632416219</v>
-      </c>
-      <c r="Q6" s="60">
-        <v>-0.23163087276473621</v>
-      </c>
-      <c r="S6" s="4"/>
-    </row>
-    <row r="7" spans="2:19" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="66" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="66"/>
-      <c r="D8" s="66"/>
-      <c r="E8" s="66"/>
-      <c r="F8" s="66"/>
-      <c r="G8" s="66"/>
-      <c r="H8" s="66"/>
-      <c r="I8" s="66"/>
-      <c r="J8" s="66"/>
-      <c r="K8" s="66"/>
-      <c r="L8" s="66"/>
-      <c r="M8" s="66"/>
-      <c r="N8" s="66"/>
-      <c r="O8" s="66"/>
-      <c r="P8" s="66"/>
-      <c r="Q8" s="66"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="B8:Q8"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25C3ECDC-F20E-4773-9F8E-9FC7ED3C0073}">
   <dimension ref="A1:V32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2752,7 +1869,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -2820,7 +1937,7 @@
         <v>1.1903486364110509</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>3</v>
       </c>
@@ -2888,7 +2005,7 @@
         <v>1.222139587123183</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>4</v>
       </c>
@@ -2956,7 +2073,7 @@
         <v>1.2126433071410041</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>5</v>
       </c>
@@ -3024,7 +2141,7 @@
         <v>1.188275801869273</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>6</v>
       </c>
@@ -3092,7 +2209,7 @@
         <v>1.2239761362433981</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>7</v>
       </c>
@@ -3160,7 +2277,7 @@
         <v>1.2345148773242749</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>8</v>
       </c>
@@ -3228,7 +2345,7 @@
         <v>1.190730903356781</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>9</v>
       </c>
@@ -3296,7 +2413,7 @@
         <v>1.207060791281843</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>10</v>
       </c>
@@ -3364,7 +2481,7 @@
         <v>1.1952535588510449</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -3432,7 +2549,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>2</v>
       </c>
@@ -3500,7 +2617,7 @@
         <v>0.50333878746192562</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>3</v>
       </c>
@@ -3568,7 +2685,7 @@
         <v>0.48648922698478297</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>4</v>
       </c>
@@ -3636,7 +2753,7 @@
         <v>0.47977949845395668</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>5</v>
       </c>
@@ -3704,7 +2821,7 @@
         <v>0.48557770624460278</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>6</v>
       </c>
@@ -3772,7 +2889,7 @@
         <v>0.51072996793889569</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>7</v>
       </c>
@@ -3840,7 +2957,7 @@
         <v>0.52263896109697938</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>8</v>
       </c>
@@ -3908,7 +3025,7 @@
         <v>0.49691709942187873</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>9</v>
       </c>
@@ -3976,7 +3093,7 @@
         <v>0.51721303161190113</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>10</v>
       </c>
@@ -4044,7 +3161,7 @@
         <v>0.51180361985093281</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
@@ -4067,7 +3184,7 @@
       <c r="U22" s="4"/>
       <c r="V22" s="4"/>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -4135,7 +3252,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>2</v>
       </c>
@@ -4203,7 +3320,7 @@
         <v>-0.18007411681755051</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>3</v>
       </c>
@@ -4271,7 +3388,7 @@
         <v>-0.26357165784328851</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>4</v>
       </c>
@@ -4339,7 +3456,7 @@
         <v>-0.26868529350546971</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>5</v>
       </c>
@@ -4407,7 +3524,7 @@
         <v>-0.2408059394250468</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>6</v>
       </c>
@@ -4475,7 +3592,7 @@
         <v>-0.21369578090810001</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>7</v>
       </c>
@@ -4543,7 +3660,7 @@
         <v>-0.18193622456181041</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>8</v>
       </c>
@@ -4611,7 +3728,7 @@
         <v>-0.19745223944941609</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>9</v>
       </c>
@@ -4679,7 +3796,7 @@
         <v>-0.15849019722071889</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>10</v>
       </c>

</xml_diff>